<commit_message>
Add NO_LABEL to groups
</commit_message>
<xml_diff>
--- a/basic-forms/forms/app/dynamic_url.xlsx
+++ b/basic-forms/forms/app/dynamic_url.xlsx
@@ -43,6 +43,7 @@
             <color rgb="FF0000FF"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">https://docs.getodk.org/form-question-types/
 </t>
@@ -105,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -232,11 +233,12 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -258,10 +260,17 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -389,41 +398,53 @@
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -532,7 +553,6 @@
           <bgColor rgb="FFFFCCCC"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -716,7 +736,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I18" activeCellId="0" sqref="I18"/>
+      <selection pane="bottomRight" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -806,7 +826,9 @@
       <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
@@ -857,7 +879,9 @@
       <c r="B12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="E12" s="1" t="s">
         <v>8</v>
       </c>
@@ -5978,44 +6002,44 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="17.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="32.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="7" t="n">
+      <c r="C2" s="8" t="n">
         <f aca="true">NOW()</f>
-        <v>45544.3717359003</v>
+        <v>45544.4530230467</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="6" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>